<commit_message>
- Add Initial function:     InitialTestItemResult()     InitialTestStepResult()  - Update DutWebScript
</commit_message>
<xml_diff>
--- a/CyberRouterATE/bin/Debug/testCondition/DutWebScript/MR9000_WebGuiScript_.xlsx
+++ b/CyberRouterATE/bin/Debug/testCondition/DutWebScript/MR9000_WebGuiScript_.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="360" windowWidth="15360" windowHeight="6240"/>
+    <workbookView xWindow="6660" yWindow="405" windowWidth="15360" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sample!$C$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sample!$C$1:$C$109</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="113">
   <si>
     <t>TEXT_BOX</t>
   </si>
@@ -417,6 +417,30 @@
   </si>
   <si>
     <t>//*[@id="widget-copyright"]/div/div[1]/a[7]</t>
+  </si>
+  <si>
+    <t>GotoConnectivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait until timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckFwVersion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckFwVersion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait until timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait for Element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -832,24 +856,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101:XFD123"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="B75:B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="60.109375" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="60.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,50 +1296,41 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="3">
-        <v>2</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
         <v>35</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="I26" s="1">
         <v>90</v>
       </c>
     </row>
@@ -1324,16 +1339,25 @@
         <v>22</v>
       </c>
       <c r="B29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" t="s">
+        <v>25</v>
       </c>
       <c r="I29" s="1">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1341,25 +1365,16 @@
         <v>22</v>
       </c>
       <c r="B30" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I30" s="1">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1367,377 +1382,383 @@
         <v>22</v>
       </c>
       <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>31</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="I32" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>55</v>
       </c>
-      <c r="I34" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="J36" s="7"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="I35" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>57</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>10</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="I38" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
         <v>91</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>10</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>92</v>
       </c>
-      <c r="I40" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:10" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="I41" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="I46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" t="s">
-        <v>100</v>
-      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+      <c r="H49" t="s">
+        <v>100</v>
+      </c>
+      <c r="I49" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B51" s="3">
+        <v>3</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" t="s">
+        <v>100</v>
+      </c>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="3">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>16</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H52" t="s">
         <v>103</v>
       </c>
-      <c r="I49" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="I52" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="3">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>101</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E53" t="s">
         <v>10</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H53" t="s">
         <v>100</v>
       </c>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="J51" s="7"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E53" t="s">
-        <v>63</v>
-      </c>
-      <c r="H53" t="s">
-        <v>64</v>
-      </c>
-      <c r="I53" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="3">
-        <v>2</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" t="s">
-        <v>63</v>
-      </c>
-      <c r="H54" t="s">
-        <v>66</v>
-      </c>
-      <c r="I54" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="3">
-        <v>3</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55" t="s">
-        <v>68</v>
-      </c>
-      <c r="I55" s="1">
-        <v>90</v>
-      </c>
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J54" s="7"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E56" t="s">
         <v>63</v>
       </c>
       <c r="H56" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I56" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" t="s">
+        <v>63</v>
+      </c>
+      <c r="H57" t="s">
+        <v>66</v>
+      </c>
+      <c r="I57" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="3">
+        <v>3</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" t="s">
+        <v>68</v>
+      </c>
+      <c r="I58" s="1">
         <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B59" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="E59" t="s">
+        <v>63</v>
       </c>
       <c r="H59" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="I59" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="3">
-        <v>2</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-      <c r="H60" t="s">
-        <v>77</v>
-      </c>
-      <c r="I60" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" s="3">
-        <v>3</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" t="s">
-        <v>78</v>
-      </c>
-      <c r="H61" t="s">
-        <v>79</v>
-      </c>
-      <c r="I61" s="1">
-        <v>90</v>
-      </c>
-      <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
       <c r="B62" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>69</v>
-      </c>
-      <c r="E62" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="H62" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="I62" s="1">
         <v>90</v>
       </c>
-      <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>71</v>
       </c>
       <c r="B63" s="3">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="1">
         <v>5</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" t="s">
-        <v>81</v>
-      </c>
-      <c r="H63" t="s">
-        <v>82</v>
-      </c>
-      <c r="I63" s="1">
-        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -1745,19 +1766,19 @@
         <v>71</v>
       </c>
       <c r="B64" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H64" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="I64" s="1">
         <v>90</v>
@@ -1768,170 +1789,170 @@
         <v>71</v>
       </c>
       <c r="B65" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>76</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
       </c>
       <c r="H65" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I65" s="1">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>69</v>
-      </c>
-      <c r="E66" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="I66" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>
       <c r="B67" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
       </c>
       <c r="H67" t="s">
-        <v>19</v>
+        <v>80</v>
+      </c>
+      <c r="I67" s="1">
+        <v>90</v>
+      </c>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="3">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" t="s">
+        <v>81</v>
+      </c>
+      <c r="H68" t="s">
+        <v>82</v>
+      </c>
+      <c r="I68" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="3">
+        <v>8</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" t="s">
+        <v>84</v>
+      </c>
+      <c r="I69" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B70" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="H70" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I70" s="1">
-        <v>90</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B71" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
       </c>
       <c r="H71" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="I71" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H72" t="s">
-        <v>79</v>
-      </c>
-      <c r="I72" s="1">
-        <v>90</v>
-      </c>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="3">
-        <v>4</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" t="s">
-        <v>69</v>
-      </c>
-      <c r="E73" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" t="s">
-        <v>80</v>
-      </c>
-      <c r="I73" s="1">
-        <v>90</v>
-      </c>
-      <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>21</v>
-      </c>
-      <c r="B74" s="3">
-        <v>5</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" t="s">
-        <v>81</v>
-      </c>
-      <c r="H74" t="s">
-        <v>82</v>
-      </c>
-      <c r="I74" s="1">
-        <v>240</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -1939,19 +1960,16 @@
         <v>21</v>
       </c>
       <c r="B75" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>83</v>
-      </c>
-      <c r="E75" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="H75" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="I75" s="1">
         <v>90</v>
@@ -1962,19 +1980,16 @@
         <v>21</v>
       </c>
       <c r="B76" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>85</v>
-      </c>
-      <c r="H76" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="I76" s="1">
-        <v>240</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -1982,19 +1997,19 @@
         <v>21</v>
       </c>
       <c r="B77" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D77" t="s">
-        <v>69</v>
-      </c>
-      <c r="E77" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="H77" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="I77" s="1">
         <v>90</v>
@@ -2005,103 +2020,294 @@
         <v>21</v>
       </c>
       <c r="B78" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>87</v>
+        <v>76</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
       </c>
       <c r="H78" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="I78" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="3">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" t="s">
+        <v>78</v>
+      </c>
+      <c r="H79" t="s">
+        <v>79</v>
+      </c>
+      <c r="I79" s="1">
+        <v>90</v>
+      </c>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="3">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" t="s">
+        <v>80</v>
+      </c>
+      <c r="I80" s="1">
+        <v>90</v>
+      </c>
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="3">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" t="s">
+        <v>81</v>
+      </c>
+      <c r="H81" t="s">
+        <v>82</v>
+      </c>
+      <c r="I81" s="1">
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B82" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
       </c>
       <c r="H82" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="I82" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B83" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E83" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D83" t="s">
+        <v>85</v>
       </c>
       <c r="H83" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="I83" s="1">
-        <v>90</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="B84" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
       </c>
       <c r="H84" t="s">
+        <v>20</v>
+      </c>
+      <c r="I84" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="3">
+        <v>11</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+      <c r="H85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D89" t="s">
+        <v>112</v>
+      </c>
+      <c r="H89" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="I89" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3">
+        <v>2</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" t="s">
+        <v>111</v>
+      </c>
+      <c r="I90" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="3">
+        <v>3</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>101</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="3">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E92" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" t="s">
+        <v>103</v>
+      </c>
+      <c r="I92" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="3">
+        <v>5</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>101</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B51 B53:B1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B54 B56:B1048576">
       <formula1>1</formula1>
       <formula2>99999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27 C44 C87:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28 C45 C96:C1048576">
       <formula1>"Set,Get,Wait,FileUpload,Refresh,ReLogin,AlertLogin,CloseWeb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C31 C24:C26 C43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C32 C44 C24 C26:C27">
       <formula1>"Set,Get,ReLogin,AlertLogin,FileUpload,Wait,Refresh"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E51 E53:E100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E54 E56:E109">
       <formula1>"TABLE,BUTTON,CHECK_BOX,TEXT_BOX,DROP_DOWN_LIST,AutoUI,RADIO_BUTTON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32:C42 C45:C86 C2:C23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C23 C33:C43 C25 C46:C95">
       <formula1>"Set,Get,Wait,Goto,FileUpload,Refresh,ReLogin,AlertLogin,CloseWeb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E101:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E110:E1048576">
       <formula1>"BUTTON,CHECK_BOX,TEXT_BOX,DROP_DOWN_LIST,RADIO_BUTTON"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>